<commit_message>
event manager delete an api
</commit_message>
<xml_diff>
--- a/ExcelConfig/pbjson/excel/基础条件表.xlsx
+++ b/ExcelConfig/pbjson/excel/基础条件表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CatClub\CatClub\ExcelConfig\pbjson\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CatClub\ExcelConfig\pbjson\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3C42F6-75F5-4587-9C6B-891A4C60F478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423B0BDB-48FD-4FAB-B597-48135CCD7DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="5370" windowWidth="19050" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18930" yWindow="3870" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#基础条件配置" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>条件编号</t>
   </si>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>拥有至少X点“猫咪集群”</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>当前时间已到达X</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -118,10 +114,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>猫咪阴谋X，目标Y已完成</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>目标人物X，拥有性格标签Y</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -287,6 +279,18 @@
   </si>
   <si>
     <t>故事进度小于等于X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>func()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拥有至少X点“隐匿度”</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>猫咪阴谋目标X已完成</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -690,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="A2:B54"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,15 +706,18 @@
     <col min="2" max="2" width="47.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>4000</v>
       </c>
@@ -718,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>4001</v>
       </c>
@@ -726,108 +733,108 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4002</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4003</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4004</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4005</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>4006</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>4007</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>4008</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>4100</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>4101</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>4102</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>4103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>4104</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>4105</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -835,7 +842,7 @@
         <v>4106</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -843,7 +850,7 @@
         <v>4107</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -851,7 +858,7 @@
         <v>4108</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -859,7 +866,7 @@
         <v>4109</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -867,7 +874,7 @@
         <v>4110</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -875,7 +882,7 @@
         <v>4111</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -883,7 +890,7 @@
         <v>4112</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -891,7 +898,7 @@
         <v>4113</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -899,7 +906,7 @@
         <v>4114</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -907,7 +914,7 @@
         <v>4115</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -931,7 +938,7 @@
         <v>4118</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -939,7 +946,7 @@
         <v>4200</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -947,7 +954,7 @@
         <v>4201</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -955,7 +962,7 @@
         <v>4202</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -963,7 +970,7 @@
         <v>4203</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -971,7 +978,7 @@
         <v>4204</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -979,7 +986,7 @@
         <v>4205</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -987,7 +994,7 @@
         <v>4206</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -995,7 +1002,7 @@
         <v>4207</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1003,7 +1010,7 @@
         <v>4208</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1011,7 +1018,7 @@
         <v>4209</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1019,7 +1026,7 @@
         <v>4210</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1027,7 +1034,7 @@
         <v>4211</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1035,7 +1042,7 @@
         <v>4300</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,7 +1050,7 @@
         <v>4301</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1051,7 +1058,7 @@
         <v>4302</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,7 +1066,7 @@
         <v>4303</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1067,7 +1074,7 @@
         <v>4304</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1075,7 +1082,7 @@
         <v>4305</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1083,7 +1090,7 @@
         <v>4400</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1091,7 +1098,7 @@
         <v>4401</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1099,7 +1106,7 @@
         <v>4402</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1107,7 +1114,7 @@
         <v>4403</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1115,7 +1122,7 @@
         <v>4500</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1123,7 +1130,7 @@
         <v>4501</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1131,7 +1138,7 @@
         <v>4502</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1173,6 +1180,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change npc manager info
</commit_message>
<xml_diff>
--- a/ExcelConfig/pbjson/excel/基础条件表.xlsx
+++ b/ExcelConfig/pbjson/excel/基础条件表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CatClub\ExcelConfig\pbjson\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CatClub\ExcelConfig\pbjson\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E36745-B715-4F4C-AE52-A01F44D4AAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D199ADC-DD50-4B3E-87BE-07BB38FBA068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8925" yWindow="5205" windowWidth="21465" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#基础条件配置" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -338,6 +338,13 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="9"/>
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
@@ -398,7 +405,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -417,6 +424,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -955,19 +968,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+    <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>4116</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>4117</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1127,7 +1140,7 @@
       <c r="A48" s="2">
         <v>4400</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1151,7 +1164,7 @@
       <c r="A51" s="2">
         <v>4403</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="7" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>